<commit_message>
cleaned up nest and unnest
</commit_message>
<xml_diff>
--- a/boyd/Boyd_CABU6(1).xlsx
+++ b/boyd/Boyd_CABU6(1).xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donbo\Documents\R_projects\CA_BU6\boyd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB5319B-1413-4559-B8D9-7AD1CD64C4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C729D2C3-AADC-4493-A24A-22D45FE5EE0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{FD967513-E3F3-4989-ACFE-6DCC63C78927}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{FD967513-E3F3-4989-ACFE-6DCC63C78927}"/>
   </bookViews>
   <sheets>
     <sheet name="pension_parameters" sheetId="1" r:id="rId1"/>
     <sheet name="SocialSecurity" sheetId="2" r:id="rId2"/>
     <sheet name="awiseries" sheetId="3" r:id="rId3"/>
+    <sheet name="bends" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
   <si>
     <t>stabbr</t>
   </si>
@@ -177,6 +178,21 @@
   </si>
   <si>
     <t xml:space="preserve"> poffass</t>
+  </si>
+  <si>
+    <t>Dollar amounts in PIA formula</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Year of eligibility; that is, the year in which a worker attains age 62, becomes disabled before age 62, or dies before attaining age 62.</t>
+  </si>
+  <si>
+    <t>Growth rate in the bends points is same as in the awi (adjusted wage index) series, but lagged 2 years. That is (I guess) because bends are for the year the person first turned 62 but awi is based on age 60???</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>second</t>
   </si>
 </sst>
 </file>
@@ -186,9 +202,9 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,8 +238,14 @@
       <color rgb="FF212121"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF212121"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,6 +261,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEEEEEE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEF4EE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,11 +307,11 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -302,6 +336,10 @@
     <xf numFmtId="10" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -621,7 +659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF9F42EE-6DDD-4C15-80B7-D8E501EEEEEB}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1072,7 +1110,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="F52" sqref="F52:F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2298,4 +2336,948 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B80D6A3-18B3-451A-A4DA-4AFBAB07A52B}">
+  <dimension ref="A2:G50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="3" width="9.109375" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1979</v>
+      </c>
+      <c r="B5" s="3">
+        <v>180</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1980</v>
+      </c>
+      <c r="B6" s="3">
+        <v>194</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1171</v>
+      </c>
+      <c r="E6" s="1">
+        <f>+B6/B5-1</f>
+        <v>7.7777777777777724E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" ref="F6:F48" si="0">+C6/C5-1</f>
+        <v>7.926267281105992E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1981</v>
+      </c>
+      <c r="B7" s="3">
+        <v>211</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1274</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" ref="E7:E48" si="1">+B7/B6-1</f>
+        <v>8.7628865979381354E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>8.7959009393680621E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1982</v>
+      </c>
+      <c r="B8" s="3">
+        <v>230</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1388</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>9.004739336492884E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>8.9481946624803799E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1983</v>
+      </c>
+      <c r="B9" s="3">
+        <v>254</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1528</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.10434782608695659</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.10086455331412103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1984</v>
+      </c>
+      <c r="B10" s="3">
+        <v>267</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1612</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="1"/>
+        <v>5.1181102362204633E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>5.4973821989528826E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1985</v>
+      </c>
+      <c r="B11" s="3">
+        <v>280</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1691</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="1"/>
+        <v>4.8689138576778923E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="0"/>
+        <v>4.9007444168734482E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1986</v>
+      </c>
+      <c r="B12" s="3">
+        <v>297</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1790</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="1"/>
+        <v>6.0714285714285721E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="0"/>
+        <v>5.8545239503252411E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1987</v>
+      </c>
+      <c r="B13" s="3">
+        <v>310</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1866</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>4.3771043771043683E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="0"/>
+        <v>4.2458100558659284E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1988</v>
+      </c>
+      <c r="B14" s="3">
+        <v>319</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1922</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="1"/>
+        <v>2.9032258064516148E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="0"/>
+        <v>3.0010718113612E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1989</v>
+      </c>
+      <c r="B15" s="3">
+        <v>339</v>
+      </c>
+      <c r="C15" s="3">
+        <v>2044</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="1"/>
+        <v>6.2695924764890387E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="0"/>
+        <v>6.347554630593133E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1990</v>
+      </c>
+      <c r="B16" s="3">
+        <v>356</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2145</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="1"/>
+        <v>5.0147492625368661E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="0"/>
+        <v>4.9412915851271944E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>1991</v>
+      </c>
+      <c r="B17" s="3">
+        <v>370</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2230</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="1"/>
+        <v>3.9325842696629199E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="0"/>
+        <v>3.9627039627039728E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>1992</v>
+      </c>
+      <c r="B18" s="3">
+        <v>387</v>
+      </c>
+      <c r="C18" s="3">
+        <v>2333</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="1"/>
+        <v>4.5945945945945921E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="0"/>
+        <v>4.6188340807174821E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1993</v>
+      </c>
+      <c r="B19" s="3">
+        <v>401</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2420</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="1"/>
+        <v>3.6175710594315236E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="0"/>
+        <v>3.7291041577368178E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>1994</v>
+      </c>
+      <c r="B20" s="3">
+        <v>422</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2545</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="1"/>
+        <v>5.2369077306733125E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="0"/>
+        <v>5.1652892561983466E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>1995</v>
+      </c>
+      <c r="B21" s="3">
+        <v>426</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2567</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="1"/>
+        <v>9.4786729857820884E-3</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="0"/>
+        <v>8.6444007858546001E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>1996</v>
+      </c>
+      <c r="B22" s="3">
+        <v>437</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2635</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="1"/>
+        <v>2.5821596244131495E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="0"/>
+        <v>2.6490066225165476E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>1997</v>
+      </c>
+      <c r="B23" s="3">
+        <v>455</v>
+      </c>
+      <c r="C23" s="3">
+        <v>2741</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="1"/>
+        <v>4.1189931350114506E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="0"/>
+        <v>4.0227703984819785E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>1998</v>
+      </c>
+      <c r="B24" s="3">
+        <v>477</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2875</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="1"/>
+        <v>4.8351648351648402E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="0"/>
+        <v>4.8887267420649305E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>1999</v>
+      </c>
+      <c r="B25" s="3">
+        <v>505</v>
+      </c>
+      <c r="C25" s="3">
+        <v>3043</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="1"/>
+        <v>5.8700209643605783E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="0"/>
+        <v>5.8434782608695723E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2000</v>
+      </c>
+      <c r="B26" s="3">
+        <v>531</v>
+      </c>
+      <c r="C26" s="3">
+        <v>3202</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="1"/>
+        <v>5.1485148514851531E-2</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="0"/>
+        <v>5.2251068024975256E-2</v>
+      </c>
+      <c r="G26" s="13">
+        <v>5.5300000000000002E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>2001</v>
+      </c>
+      <c r="B27" s="3">
+        <v>561</v>
+      </c>
+      <c r="C27" s="3">
+        <v>3381</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="1"/>
+        <v>5.6497175141242861E-2</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="0"/>
+        <v>5.5902560899437903E-2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>2.3900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2002</v>
+      </c>
+      <c r="B28" s="3">
+        <v>592</v>
+      </c>
+      <c r="C28" s="3">
+        <v>3567</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="1"/>
+        <v>5.525846702317283E-2</v>
+      </c>
+      <c r="F28" s="13">
+        <f t="shared" si="0"/>
+        <v>5.501330967169471E-2</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>2003</v>
+      </c>
+      <c r="B29" s="3">
+        <v>606</v>
+      </c>
+      <c r="C29" s="3">
+        <v>3653</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="1"/>
+        <v>2.3648648648648685E-2</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="0"/>
+        <v>2.4109896271376607E-2</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2.4400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>2004</v>
+      </c>
+      <c r="B30" s="3">
+        <v>612</v>
+      </c>
+      <c r="C30" s="3">
+        <v>3689</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="1"/>
+        <v>9.9009900990099098E-3</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="0"/>
+        <v>9.8549137695045363E-3</v>
+      </c>
+      <c r="G30" s="1">
+        <v>4.65E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>2005</v>
+      </c>
+      <c r="B31" s="3">
+        <v>627</v>
+      </c>
+      <c r="C31" s="3">
+        <v>3779</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="1"/>
+        <v>2.450980392156854E-2</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="0"/>
+        <v>2.4396855516400029E-2</v>
+      </c>
+      <c r="G31" s="1">
+        <v>3.6600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>2006</v>
+      </c>
+      <c r="B32" s="3">
+        <v>656</v>
+      </c>
+      <c r="C32" s="3">
+        <v>3955</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" si="1"/>
+        <v>4.6251993620414655E-2</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="0"/>
+        <v>4.6573167504630808E-2</v>
+      </c>
+      <c r="G32" s="1">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>2007</v>
+      </c>
+      <c r="B33" s="3">
+        <v>680</v>
+      </c>
+      <c r="C33" s="3">
+        <v>4100</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" si="1"/>
+        <v>3.6585365853658569E-2</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="0"/>
+        <v>3.6662452591656125E-2</v>
+      </c>
+      <c r="G33" s="1">
+        <v>4.5400000000000003E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>2008</v>
+      </c>
+      <c r="B34" s="3">
+        <v>711</v>
+      </c>
+      <c r="C34" s="3">
+        <v>4288</v>
+      </c>
+      <c r="E34" s="1">
+        <f t="shared" si="1"/>
+        <v>4.5588235294117707E-2</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" si="0"/>
+        <v>4.5853658536585407E-2</v>
+      </c>
+      <c r="G34" s="1">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>2009</v>
+      </c>
+      <c r="B35" s="3">
+        <v>744</v>
+      </c>
+      <c r="C35" s="3">
+        <v>4483</v>
+      </c>
+      <c r="E35" s="1">
+        <f t="shared" si="1"/>
+        <v>4.6413502109704741E-2</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="0"/>
+        <v>4.5475746268656803E-2</v>
+      </c>
+      <c r="G35" s="1">
+        <v>-1.5100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>2010</v>
+      </c>
+      <c r="B36" s="3">
+        <v>761</v>
+      </c>
+      <c r="C36" s="3">
+        <v>4586</v>
+      </c>
+      <c r="E36" s="1">
+        <f t="shared" si="1"/>
+        <v>2.2849462365591489E-2</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2975685924603972E-2</v>
+      </c>
+      <c r="G36" s="1">
+        <v>2.3599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>2011</v>
+      </c>
+      <c r="B37" s="3">
+        <v>749</v>
+      </c>
+      <c r="C37" s="3">
+        <v>4517</v>
+      </c>
+      <c r="E37" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.5768725361366642E-2</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.5045791539467945E-2</v>
+      </c>
+      <c r="G37" s="1">
+        <v>3.1300000000000001E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>2012</v>
+      </c>
+      <c r="B38" s="3">
+        <v>767</v>
+      </c>
+      <c r="C38" s="3">
+        <v>4624</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" si="1"/>
+        <v>2.4032042723631575E-2</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3688288687181869E-2</v>
+      </c>
+      <c r="G38" s="1">
+        <v>3.1199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>2013</v>
+      </c>
+      <c r="B39" s="3">
+        <v>791</v>
+      </c>
+      <c r="C39" s="3">
+        <v>4768</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" si="1"/>
+        <v>3.1290743155149903E-2</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="0"/>
+        <v>3.114186851211076E-2</v>
+      </c>
+      <c r="G39" s="1">
+        <v>1.2800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>2014</v>
+      </c>
+      <c r="B40" s="3">
+        <v>816</v>
+      </c>
+      <c r="C40" s="3">
+        <v>4917</v>
+      </c>
+      <c r="E40" s="1">
+        <f t="shared" si="1"/>
+        <v>3.1605562579013924E-2</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="0"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="G40" s="1">
+        <v>3.5499999999999997E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>2015</v>
+      </c>
+      <c r="B41" s="3">
+        <v>826</v>
+      </c>
+      <c r="C41" s="3">
+        <v>4980</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" si="1"/>
+        <v>1.225490196078427E-2</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="0"/>
+        <v>1.281269066503965E-2</v>
+      </c>
+      <c r="G41" s="1">
+        <v>3.4799999999999998E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>2016</v>
+      </c>
+      <c r="B42" s="3">
+        <v>856</v>
+      </c>
+      <c r="C42" s="3">
+        <v>5157</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" si="1"/>
+        <v>3.6319612590798966E-2</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="0"/>
+        <v>3.5542168674698837E-2</v>
+      </c>
+      <c r="G42" s="1">
+        <v>1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>2017</v>
+      </c>
+      <c r="B43" s="3">
+        <v>885</v>
+      </c>
+      <c r="C43" s="3">
+        <v>5336</v>
+      </c>
+      <c r="E43" s="1">
+        <f t="shared" si="1"/>
+        <v>3.3878504672897103E-2</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="0"/>
+        <v>3.4710102772929963E-2</v>
+      </c>
+      <c r="G43" s="1">
+        <v>3.4500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>2018</v>
+      </c>
+      <c r="B44" s="3">
+        <v>895</v>
+      </c>
+      <c r="C44" s="3">
+        <v>5397</v>
+      </c>
+      <c r="E44" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1299435028248483E-2</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1431784107946097E-2</v>
+      </c>
+      <c r="G44" s="1">
+        <v>3.6200000000000003E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>2019</v>
+      </c>
+      <c r="B45" s="3">
+        <v>926</v>
+      </c>
+      <c r="C45" s="3">
+        <v>5583</v>
+      </c>
+      <c r="E45" s="1">
+        <f t="shared" si="1"/>
+        <v>3.4636871508379796E-2</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="0"/>
+        <v>3.4463590883824446E-2</v>
+      </c>
+      <c r="G45" s="1">
+        <v>3.7499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>2020</v>
+      </c>
+      <c r="B46" s="3">
+        <v>960</v>
+      </c>
+      <c r="C46" s="3">
+        <v>5785</v>
+      </c>
+      <c r="E46" s="1">
+        <f t="shared" si="1"/>
+        <v>3.6717062634989306E-2</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="0"/>
+        <v>3.6181264553107662E-2</v>
+      </c>
+      <c r="G46" s="13">
+        <v>2.8299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>2021</v>
+      </c>
+      <c r="B47" s="3">
+        <v>996</v>
+      </c>
+      <c r="C47" s="3">
+        <v>6002</v>
+      </c>
+      <c r="E47" s="1">
+        <f t="shared" si="1"/>
+        <v>3.7500000000000089E-2</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="0"/>
+        <v>3.7510803802938586E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>2022</v>
+      </c>
+      <c r="B48" s="3">
+        <v>1024</v>
+      </c>
+      <c r="C48" s="3">
+        <v>6172</v>
+      </c>
+      <c r="E48" s="1">
+        <f t="shared" si="1"/>
+        <v>2.8112449799196693E-2</v>
+      </c>
+      <c r="F48" s="13">
+        <f t="shared" si="0"/>
+        <v>2.8323892035988063E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added defined contribution plan
</commit_message>
<xml_diff>
--- a/boyd/Boyd_CABU6(1).xlsx
+++ b/boyd/Boyd_CABU6(1).xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donbo\Documents\R_projects\CA_BU6\boyd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C729D2C3-AADC-4493-A24A-22D45FE5EE0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB6022C-BDDE-456E-958F-D07574215311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{FD967513-E3F3-4989-ACFE-6DCC63C78927}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{FD967513-E3F3-4989-ACFE-6DCC63C78927}"/>
   </bookViews>
   <sheets>
-    <sheet name="pension_parameters" sheetId="1" r:id="rId1"/>
-    <sheet name="SocialSecurity" sheetId="2" r:id="rId2"/>
+    <sheet name="retplan_parameters" sheetId="1" r:id="rId1"/>
+    <sheet name="plan_notes" sheetId="5" r:id="rId2"/>
     <sheet name="awiseries" sheetId="3" r:id="rId3"/>
     <sheet name="bends" sheetId="4" r:id="rId4"/>
+    <sheet name="SocialSecurity" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="82">
   <si>
     <t>stabbr</t>
   </si>
@@ -54,18 +55,9 @@
     <t xml:space="preserve"> aor_min</t>
   </si>
   <si>
-    <t xml:space="preserve"> maxpct</t>
-  </si>
-  <si>
     <t xml:space="preserve"> cola</t>
   </si>
   <si>
-    <t xml:space="preserve"> compound</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fasperiod</t>
-  </si>
-  <si>
     <t xml:space="preserve"> socsec</t>
   </si>
   <si>
@@ -102,21 +94,9 @@
     <t xml:space="preserve"> poffa</t>
   </si>
   <si>
-    <t>eec_exclude</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> benfactor_normal</t>
-  </si>
-  <si>
-    <t>benfactor_min</t>
-  </si>
-  <si>
     <t>MA</t>
   </si>
   <si>
-    <t>eec_rate</t>
-  </si>
-  <si>
     <t>Links</t>
   </si>
   <si>
@@ -193,6 +173,117 @@
   </si>
   <si>
     <t>second</t>
+  </si>
+  <si>
+    <t>ss_covered</t>
+  </si>
+  <si>
+    <t>bend1</t>
+  </si>
+  <si>
+    <t>bend2</t>
+  </si>
+  <si>
+    <t>db_covered</t>
+  </si>
+  <si>
+    <t>dc_covered</t>
+  </si>
+  <si>
+    <t>dc_ror</t>
+  </si>
+  <si>
+    <t>db_benfactor_min</t>
+  </si>
+  <si>
+    <t>db_aor_normal</t>
+  </si>
+  <si>
+    <t>db_aor_min</t>
+  </si>
+  <si>
+    <t>db_max_benpct</t>
+  </si>
+  <si>
+    <t>db_cola</t>
+  </si>
+  <si>
+    <t>db_cola_compound</t>
+  </si>
+  <si>
+    <t>db_fasperiod</t>
+  </si>
+  <si>
+    <t>db_eec_rate</t>
+  </si>
+  <si>
+    <t>db_eec_exclude</t>
+  </si>
+  <si>
+    <t>db_source</t>
+  </si>
+  <si>
+    <t>dc_eec_rate</t>
+  </si>
+  <si>
+    <t>dc_erc_rate</t>
+  </si>
+  <si>
+    <t>private</t>
+  </si>
+  <si>
+    <t>dc555</t>
+  </si>
+  <si>
+    <t>db_benfactor_normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> benfactor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rpypp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cola_compound</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eec</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>VERIFY that FAS=1 year for poffa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLA for all 3 is % starting in 2nd year after retirement. </t>
+  </si>
+  <si>
+    <t>Cumulative adjustment can't be more than cumulative change in CPI since retirement</t>
+  </si>
+  <si>
+    <t>https://www.calpers.ca.gov/page/newsroom/calpers-news/2017/board-adopts-new-rates-state-school-employers</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>unknown</t>
   </si>
 </sst>
 </file>
@@ -307,7 +398,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -340,6 +431,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -358,6 +458,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>255238</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>43535</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC706BDE-E485-446B-BB05-58BBCA5872AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="182880"/>
+          <a:ext cx="15495238" cy="2238095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -657,370 +806,492 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF9F42EE-6DDD-4C15-80B7-D8E501EEEEEB}">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="8.88671875" style="1"/>
-    <col min="5" max="5" width="8.88671875" style="2"/>
-    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="1"/>
+    <col min="11" max="11" width="8.88671875" style="2"/>
+    <col min="19" max="19" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:20" s="14" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="D1" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="R1" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="S1" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="T1" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="K2" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L2">
+        <v>57</v>
+      </c>
+      <c r="M2">
+        <v>50</v>
+      </c>
+      <c r="N2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2">
+        <v>0.02</v>
+      </c>
+      <c r="P2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q2">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="E2" s="2">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="F2">
-        <v>57</v>
-      </c>
-      <c r="G2">
-        <v>50</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2">
-        <v>0.02</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2">
-        <v>3</v>
-      </c>
-      <c r="L2">
+      <c r="R2">
         <v>0.13</v>
       </c>
-      <c r="M2" s="3">
+      <c r="S2" s="3">
         <f>863*12</f>
         <v>10356</v>
       </c>
-      <c r="N2" t="b">
+      <c r="T2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="b">
         <v>0</v>
       </c>
-      <c r="O2" t="s">
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="K3" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L3">
+        <v>55</v>
+      </c>
+      <c r="M3">
+        <v>50</v>
+      </c>
+      <c r="N3">
+        <v>0.9</v>
+      </c>
+      <c r="O3">
+        <v>0.02</v>
+      </c>
+      <c r="P3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3">
+        <v>3</v>
+      </c>
+      <c r="R3">
+        <v>0.12</v>
+      </c>
+      <c r="S3" s="3">
+        <f t="shared" ref="S3:S4" si="0">863*12</f>
+        <v>10356</v>
+      </c>
+      <c r="T3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="L4">
+        <v>50</v>
+      </c>
+      <c r="M4">
+        <v>50</v>
+      </c>
+      <c r="N4">
+        <v>0.9</v>
+      </c>
+      <c r="O4">
+        <v>0.02</v>
+      </c>
+      <c r="P4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>0.11</v>
+      </c>
+      <c r="S4" s="3">
+        <f t="shared" si="0"/>
+        <v>10356</v>
+      </c>
+      <c r="T4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="K6" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L6">
+        <v>57</v>
+      </c>
+      <c r="M6">
+        <v>50</v>
+      </c>
+      <c r="N6" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="O6">
         <v>0.02</v>
       </c>
-      <c r="E3" s="2">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="F3">
-        <v>55</v>
-      </c>
-      <c r="G3">
-        <v>50</v>
-      </c>
-      <c r="H3">
-        <v>0.9</v>
-      </c>
-      <c r="I3">
-        <v>0.02</v>
-      </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3">
+      <c r="P6" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q6">
         <v>3</v>
       </c>
-      <c r="L3">
-        <v>0.12</v>
-      </c>
-      <c r="M3" s="3">
-        <f t="shared" ref="M3:M4" si="0">863*12</f>
-        <v>10356</v>
-      </c>
-      <c r="N3" t="b">
-        <v>0</v>
-      </c>
-      <c r="O3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="F4">
-        <v>50</v>
-      </c>
-      <c r="G4">
-        <v>50</v>
-      </c>
-      <c r="H4">
-        <v>0.9</v>
-      </c>
-      <c r="I4">
-        <v>0.02</v>
-      </c>
-      <c r="J4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>0.11</v>
-      </c>
-      <c r="M4" s="3">
-        <f t="shared" si="0"/>
-        <v>10356</v>
-      </c>
-      <c r="N4" t="b">
-        <v>0</v>
-      </c>
-      <c r="O4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="E6" s="2">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="F6">
-        <v>57</v>
-      </c>
-      <c r="G6">
-        <v>50</v>
-      </c>
-      <c r="H6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6">
-        <v>0.02</v>
-      </c>
-      <c r="J6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6">
-        <v>3</v>
-      </c>
-      <c r="L6">
+      <c r="R6">
         <v>0.13</v>
       </c>
-      <c r="M6" s="3">
+      <c r="S6" s="3">
         <f>863*12</f>
         <v>10356</v>
       </c>
-      <c r="N6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="1">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
         <v>0.02</v>
       </c>
-      <c r="E7" s="2">
+      <c r="K7" s="2">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F7">
+      <c r="L7">
         <v>55</v>
       </c>
-      <c r="G7">
+      <c r="M7">
         <v>50</v>
       </c>
-      <c r="H7">
+      <c r="N7">
         <v>0.9</v>
       </c>
-      <c r="I7">
+      <c r="O7">
         <v>0.02</v>
       </c>
-      <c r="J7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7">
+      <c r="P7" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q7">
         <v>3</v>
       </c>
-      <c r="L7">
+      <c r="R7">
         <v>0.12</v>
       </c>
-      <c r="M7" s="3">
-        <f t="shared" ref="M7:M8" si="1">863*12</f>
+      <c r="S7" s="3">
+        <f t="shared" ref="S7:S8" si="1">863*12</f>
         <v>10356</v>
       </c>
-      <c r="N7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="1">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
         <v>0.02</v>
       </c>
-      <c r="E8" s="2">
+      <c r="K8" s="2">
         <v>0.03</v>
       </c>
-      <c r="F8">
+      <c r="L8">
         <v>50</v>
       </c>
-      <c r="G8">
+      <c r="M8">
         <v>50</v>
       </c>
-      <c r="H8">
+      <c r="N8">
         <v>0.9</v>
       </c>
-      <c r="I8">
+      <c r="O8">
         <v>0.02</v>
       </c>
-      <c r="J8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8">
+      <c r="P8" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q8">
         <v>1</v>
       </c>
-      <c r="L8">
+      <c r="R8">
         <v>0.11</v>
       </c>
-      <c r="M8" s="3">
+      <c r="S8" s="3">
         <f t="shared" si="1"/>
         <v>10356</v>
       </c>
-      <c r="N8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="S9" s="3"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="S10" s="3"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="S11" s="3"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S12" s="3"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0.05</v>
+      </c>
+      <c r="H14">
+        <v>0.05</v>
+      </c>
+      <c r="I14">
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>
@@ -1029,76 +1300,247 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8881CF-46F0-46BA-A944-5CC6693A7320}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AE02BD-E093-44F3-9AF2-CAC8D5B58FD0}">
+  <dimension ref="B16:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B24" sqref="B24:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="48.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.88671875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="79.33203125" style="5" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>34</v>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" t="s">
+        <v>69</v>
+      </c>
+      <c r="I16" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K16" t="s">
+        <v>70</v>
+      </c>
+      <c r="L16" t="s">
+        <v>71</v>
+      </c>
+      <c r="M16" t="s">
+        <v>6</v>
+      </c>
+      <c r="N16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F17">
+        <v>0.02</v>
+      </c>
+      <c r="G17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17">
+        <v>57</v>
+      </c>
+      <c r="I17">
+        <v>55</v>
+      </c>
+      <c r="J17">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="K17">
+        <v>3</v>
+      </c>
+      <c r="N17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F18">
+        <v>0.02</v>
+      </c>
+      <c r="G18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18">
+        <v>57</v>
+      </c>
+      <c r="I18">
+        <v>55</v>
+      </c>
+      <c r="J18">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="K18">
+        <v>3</v>
+      </c>
+      <c r="N18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19">
+        <v>0.03</v>
+      </c>
+      <c r="F19">
+        <v>0.02</v>
+      </c>
+      <c r="G19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19">
+        <v>50</v>
+      </c>
+      <c r="I19">
+        <v>50</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>3</v>
+      </c>
+      <c r="N19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20">
+        <v>0.02</v>
+      </c>
+      <c r="F20">
+        <v>0.02</v>
+      </c>
+      <c r="G20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20">
+        <v>57</v>
+      </c>
+      <c r="I20">
+        <v>55</v>
+      </c>
+      <c r="N20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F21">
+        <v>0.02</v>
+      </c>
+      <c r="G21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21">
+        <v>57</v>
+      </c>
+      <c r="I21">
+        <v>55</v>
+      </c>
+      <c r="N21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{D67D1C14-93D1-4B44-BD72-B79E0C298057}"/>
-    <hyperlink ref="A4" r:id="rId2" xr:uid="{56B1308A-DBBC-47B0-99EA-97A8AF0105FF}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{4F32088B-4F42-4235-94FA-A09966723C00}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{DCDFA4DB-E143-48C9-8A7B-068F47C90C01}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1120,24 +1562,24 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1154,7 +1596,7 @@
         <v>2799.16</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2342,8 +2784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B80D6A3-18B3-451A-A4DA-4AFBAB07A52B}">
   <dimension ref="A2:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2353,32 +2795,32 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -3274,10 +3716,84 @@
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8881CF-46F0-46BA-A944-5CC6693A7320}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="48.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.88671875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="79.33203125" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{D67D1C14-93D1-4B44-BD72-B79E0C298057}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{56B1308A-DBBC-47B0-99EA-97A8AF0105FF}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{4F32088B-4F42-4235-94FA-A09966723C00}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{DCDFA4DB-E143-48C9-8A7B-068F47C90C01}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added massachusetts, improved calcs
</commit_message>
<xml_diff>
--- a/boyd/Boyd_CABU6(1).xlsx
+++ b/boyd/Boyd_CABU6(1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donbo\Documents\R_projects\CA_BU6\boyd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD5DC3D-F380-4515-AD79-6630C012DB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FB779E-ED2E-434E-9928-D60D6DB40F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{FD967513-E3F3-4989-ACFE-6DCC63C78927}"/>
   </bookViews>
@@ -18,6 +18,11 @@
     <sheet name="awiseries" sheetId="3" r:id="rId3"/>
     <sheet name="bends" sheetId="4" r:id="rId4"/>
     <sheet name="SocialSecurity" sheetId="2" r:id="rId5"/>
+    <sheet name="California" sheetId="6" r:id="rId6"/>
+    <sheet name="Massachusetts" sheetId="7" r:id="rId7"/>
+    <sheet name="MA_20_50" sheetId="9" r:id="rId8"/>
+    <sheet name="MA_examples" sheetId="8" r:id="rId9"/>
+    <sheet name="Sheet5" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="127">
   <si>
     <t>stabbr</t>
   </si>
@@ -73,9 +78,6 @@
     <t xml:space="preserve"> pepra</t>
   </si>
   <si>
-    <t>Inf</t>
-  </si>
-  <si>
     <t xml:space="preserve"> TRUE</t>
   </si>
   <si>
@@ -205,9 +207,6 @@
     <t>db_max_benpct</t>
   </si>
   <si>
-    <t>db_cola</t>
-  </si>
-  <si>
     <t>db_cola_compound</t>
   </si>
   <si>
@@ -232,9 +231,6 @@
     <t>private</t>
   </si>
   <si>
-    <t>dc555</t>
-  </si>
-  <si>
     <t>db_benfactor_normal</t>
   </si>
   <si>
@@ -286,10 +282,229 @@
     <t>unknown</t>
   </si>
   <si>
-    <t>dc556</t>
-  </si>
-  <si>
     <t>dc666p5</t>
+  </si>
+  <si>
+    <t>dc665</t>
+  </si>
+  <si>
+    <t>https://www.mass.gov/service-details/how-to-calculate-your-estimated-pension-benefits-msrb</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If you are a member of the State Police Department, a judge, a correction officer seeking a "20/50" retirement, or would like an estimate for a Section 10(2) (termination allowance) or disability retirement, please contact the retirement board for more information.</t>
+  </si>
+  <si>
+    <t>new hire</t>
+  </si>
+  <si>
+    <t>prior</t>
+  </si>
+  <si>
+    <t>major</t>
+  </si>
+  <si>
+    <t>Group classification</t>
+  </si>
+  <si>
+    <t>https://www.mass.gov/service-details/group-classification-overview-msrb</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Group One
+Members are officials and general employees including clerical, administrative and technical workers, laborers, mechanics, and all others not otherwise classified.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group Three
+Members are exclusively State Police officers.
+Any member of the State Police who has at least 20 years of creditable service with the State Police may elect to retire at any age prior to age 55. State Police officers should contact the State Board of Retirement for more information with regard to their retirement benefits. </t>
+  </si>
+  <si>
+    <t>For members entering service before April 2, 2012:
+To be eligible to retire, the member must meet one of the following two conditions on their projected date of retirement:
+- Member has 20 years of full-time creditable service at any age, or
+- Member has attained age 55 with 10 years creditable service</t>
+  </si>
+  <si>
+    <t>For members entering service on and after April 2, 2012:
+- All members must have a minimum of 10 years creditable service
+- Members in Group 1 must be a minimum of 60 years of age
+- Members in Group 2 must be a minimum of 55 years of age
+- Members in Group 4 must be a minimum of 50 years of age</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Members entering service before April 2, 2012 should enter the estimated average of your highest thirty-six (36) consecutive months of annual regular compensation.</t>
+  </si>
+  <si>
+    <t>FAS notes</t>
+  </si>
+  <si>
+    <t>Tier notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Members entering service on or after April 2, 2012 should enter the estimated average of your highest sixty (60) consecutive months of annual regular compensation.</t>
+  </si>
+  <si>
+    <t>https://www.mass.gov/service-details/retirement-pension-estimator</t>
+  </si>
+  <si>
+    <t>Pre 2012</t>
+  </si>
+  <si>
+    <t>Group 2; Group 4 gives the same</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> Group Two
+Members in this group include probation officers, court officers, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>certain correctional positions whose major duties require them to have the care, custody, instruction or supervision of prisoners</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and certain positions who provide direct care, custody, instruction or supervision of persons with mental illness or developmental disabilities. ...Those seeking Group 2 classification must be at least 55 years of age to be considered;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> Group Four
+Members include certain public safety officers and officials, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>correction officers and certain other correction positions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and parole officers or parole supervisors. ...Those seeking Group 4 classification must be at least 45 years old to be considered.</t>
+    </r>
+  </si>
+  <si>
+    <t>Employee contributions</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> The classification of some or all your creditable service increases the age factor used to calculate a retirement allowance, which will increase your eventual benefit.  For example, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>five years are added to one’s age for Group 2 and ten years for Group 4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Age for purposes of retirement</t>
+  </si>
+  <si>
+    <t>https://www.ncsl.org/documents/employ/pension-public-safety-table-8-6-12.pdf</t>
+  </si>
+  <si>
+    <t>NCSL doc suggests Cos are Group 4</t>
+  </si>
+  <si>
+    <t>http://www.mcofu.com/</t>
+  </si>
+  <si>
+    <t>Union</t>
+  </si>
+  <si>
+    <t>COLA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The COLA is a Cost-of-Living Adjustment for eligible retired state employees receiving a pension. A COLA is handled by the Legislature, which includes Senators, Representatives and the Governor. Each year, they may or may not recommend a COLA amount to include in the state's annual budget. For FY 2021, the recommendation by the Governor, the House, and the Senate was a 3% increase on the first $13,000 of a member's annual pension benefit. https://www.mass.gov/service-details/cola-cost-of-living-adjustment-updates-msrb</t>
+  </si>
+  <si>
+    <t>http://www.massretirees.com/</t>
+  </si>
+  <si>
+    <t>An FY22 COLA will represent the 23rd consecutive year in which a COLA has been paid to State and Teacher retirees. The current COLA base of $13,000 was established in 2011 and is the focus of ongoing efforts to incrementally increase the amount.   ... With very few exceptions, nearly every local retirement board has also approved a 3% COLA in each of the past 23 years. http://www.massretirees.com/article/issues/cola/fy22-cola-marks-23-years-increases  http://www.massretirees.com/article/issues/cola/cola-base-and-its-history</t>
+  </si>
+  <si>
+    <t>db_cola_type</t>
+  </si>
+  <si>
+    <t>legislative</t>
+  </si>
+  <si>
+    <t>db_cola_rate</t>
+  </si>
+  <si>
+    <t>db_cola_base</t>
+  </si>
+  <si>
+    <t>fixed</t>
+  </si>
+  <si>
+    <t>db_eec_base1</t>
+  </si>
+  <si>
+    <t>db_eec_rate1</t>
+  </si>
+  <si>
+    <t>db_eec_rate2</t>
+  </si>
+  <si>
+    <t>rate 1 applies to first base1 of wages, then rate2 applies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.massretirees.com/article/issues/social-security/breaking-news-wep-gpo</t>
+  </si>
+  <si>
+    <t>Social Security</t>
+  </si>
+  <si>
+    <t>https://www.mcla.edu/Assets/MCLA-Files/Administrative-Offices/HR/GS-Perc-forms/MSERS_presentation.pdf</t>
+  </si>
+  <si>
+    <t>https://malegislature.gov/Laws/GeneralLaws/PartI/TitleIV/Chapter32/Section1</t>
+  </si>
+  <si>
+    <t>dc664</t>
+  </si>
+  <si>
+    <t>Additional CA options below here</t>
   </si>
 </sst>
 </file>
@@ -301,7 +516,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -340,6 +555,14 @@
       <sz val="10"/>
       <color rgb="FF212121"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -404,7 +627,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -446,6 +669,18 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -504,6 +739,329 @@
         <a:xfrm>
           <a:off x="609600" y="182880"/>
           <a:ext cx="15495238" cy="2238095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1272540</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>2739</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E564021E-8F88-4DCE-BB49-6C230C0AF657}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12809220" y="4861560"/>
+          <a:ext cx="3581400" cy="3005019"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1203960</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>134574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>216377</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>26044</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E24AC7F-B180-4381-B669-287CD8D8F6CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16322040" y="4706574"/>
+          <a:ext cx="3104357" cy="2451790"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>655320</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>60665</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>174978</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>132681</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{916C6EA7-87E3-4DD4-9188-5CC4EF2CF221}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7780020" y="10301945"/>
+          <a:ext cx="10995378" cy="3363856"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>545241</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01AE58B3-2674-405B-B580-FFD2ED539FAA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="365760"/>
+          <a:ext cx="6031641" cy="3444240"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>197722</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>162851</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA62D9A6-23FE-4550-8CF4-715F99636F54}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="175260" y="1844040"/>
+          <a:ext cx="3680062" cy="2525051"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>284938</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>21893</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8AA24A1-395B-4115-B856-32163C3CF755}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="114300" y="4442460"/>
+          <a:ext cx="5047438" cy="3809033"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>15241</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>65153</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>52849</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6666E85D-7DF1-4CF6-9408-DD7636B9794F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15241" y="8294753"/>
+          <a:ext cx="4366260" cy="2548016"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -812,204 +1370,174 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF9F42EE-6DDD-4C15-80B7-D8E501EEEEEB}">
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomRight" activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="10" max="10" width="8.88671875" style="1"/>
     <col min="11" max="11" width="8.88671875" style="2"/>
-    <col min="19" max="19" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="14" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="T1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" s="14" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D2" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="14" t="s">
+      <c r="G2" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" s="14" t="s">
+      <c r="J2" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="L2" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="T2" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="U2" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="V2" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="W2" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="K3" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L3">
         <v>50</v>
       </c>
-      <c r="J1" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="K1" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="P1" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q1" s="14" t="s">
+      <c r="M3">
         <v>57</v>
       </c>
-      <c r="R1" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="S1" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="T1" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="b">
+      <c r="N3" s="3">
+        <v>1000000000</v>
+      </c>
+      <c r="O3" t="s">
+        <v>116</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="Q3">
         <v>0</v>
       </c>
-      <c r="F2" t="b">
+      <c r="R3" t="s">
+        <v>11</v>
+      </c>
+      <c r="S3">
+        <v>3</v>
+      </c>
+      <c r="T3" s="24">
         <v>0</v>
       </c>
-      <c r="J2" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="K2" s="2">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="L2">
-        <v>57</v>
-      </c>
-      <c r="M2">
-        <v>50</v>
-      </c>
-      <c r="N2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2">
-        <v>0.02</v>
-      </c>
-      <c r="P2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q2">
-        <v>3</v>
-      </c>
-      <c r="R2">
-        <v>0.13</v>
-      </c>
-      <c r="S2" s="3">
+      <c r="U3" s="3">
         <f>863*12</f>
         <v>10356</v>
       </c>
-      <c r="T2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="V3" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="W3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="K3" s="2">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="L3">
-        <v>55</v>
-      </c>
-      <c r="M3">
-        <v>50</v>
-      </c>
-      <c r="N3">
-        <v>0.9</v>
-      </c>
-      <c r="O3">
-        <v>0.02</v>
-      </c>
-      <c r="P3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q3">
-        <v>3</v>
-      </c>
-      <c r="R3">
-        <v>0.12</v>
-      </c>
-      <c r="S3" s="3">
-        <f t="shared" ref="S3:S4" si="0">863*12</f>
-        <v>10356</v>
-      </c>
-      <c r="T3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -1017,348 +1545,469 @@
       <c r="F4" t="b">
         <v>0</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="2">
         <v>0.02</v>
       </c>
       <c r="K4" s="2">
-        <v>0.03</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="L4">
         <v>50</v>
       </c>
       <c r="M4">
+        <v>55</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="O4" t="s">
+        <v>116</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4" t="s">
+        <v>11</v>
+      </c>
+      <c r="S4">
+        <v>3</v>
+      </c>
+      <c r="T4" s="24">
+        <v>0</v>
+      </c>
+      <c r="U4" s="3">
+        <f t="shared" ref="U4:U5" si="0">863*12</f>
+        <v>10356</v>
+      </c>
+      <c r="V4" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="W4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="L5">
         <v>50</v>
       </c>
-      <c r="N4">
+      <c r="M5">
+        <v>50</v>
+      </c>
+      <c r="N5" s="1">
         <v>0.9</v>
       </c>
-      <c r="O4">
+      <c r="O5" t="s">
+        <v>116</v>
+      </c>
+      <c r="P5" s="1">
         <v>0.02</v>
       </c>
-      <c r="P4" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q4">
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5" t="s">
+        <v>11</v>
+      </c>
+      <c r="S5">
         <v>1</v>
       </c>
-      <c r="R4">
-        <v>0.11</v>
-      </c>
-      <c r="S4" s="3">
+      <c r="T5" s="24">
+        <v>0</v>
+      </c>
+      <c r="U5" s="3">
         <f t="shared" si="0"/>
         <v>10356</v>
       </c>
-      <c r="T4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="V5" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="W5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="J6" s="2"/>
+      <c r="N6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="V6" s="1"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="b">
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="b">
         <v>0</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J7" s="2">
         <v>0.02</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K7" s="2">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="L6">
+      <c r="L7">
+        <v>50</v>
+      </c>
+      <c r="M7">
         <v>57</v>
       </c>
-      <c r="M6">
-        <v>50</v>
-      </c>
-      <c r="N6" t="s">
+      <c r="N7" s="3">
+        <v>1000000000</v>
+      </c>
+      <c r="O7" t="s">
+        <v>116</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7" t="s">
         <v>11</v>
       </c>
-      <c r="O6">
-        <v>0.02</v>
-      </c>
-      <c r="P6" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q6">
+      <c r="S7">
         <v>3</v>
       </c>
-      <c r="R6">
-        <v>0.13</v>
-      </c>
-      <c r="S6" s="3">
+      <c r="T7" s="24">
+        <v>0</v>
+      </c>
+      <c r="U7" s="3">
         <f>863*12</f>
         <v>10356</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="V7" s="1">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="J10" s="2"/>
+      <c r="U10" s="3"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="K11" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L11">
+        <v>50</v>
+      </c>
+      <c r="M11">
+        <v>57</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="O11" t="s">
+        <v>113</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>13000</v>
+      </c>
+      <c r="R11" t="s">
+        <v>11</v>
+      </c>
+      <c r="S11">
+        <v>5</v>
+      </c>
+      <c r="T11" s="24">
+        <v>0.09</v>
+      </c>
+      <c r="U11" s="3">
+        <v>30000</v>
+      </c>
+      <c r="V11" s="1">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="I15" s="2">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="K20" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L20">
+        <v>50</v>
+      </c>
+      <c r="M20">
+        <v>55</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="O20" t="s">
+        <v>116</v>
+      </c>
+      <c r="P20" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20" t="s">
+        <v>11</v>
+      </c>
+      <c r="S20">
+        <v>3</v>
+      </c>
+      <c r="T20" s="24">
+        <v>0</v>
+      </c>
+      <c r="U20" s="3">
+        <f t="shared" ref="U20:U21" si="1">863*12</f>
+        <v>10356</v>
+      </c>
+      <c r="V20" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
         <v>38</v>
       </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="b">
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="b">
         <v>0</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J21" s="2">
         <v>0.02</v>
       </c>
-      <c r="K7" s="2">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="L7">
-        <v>55</v>
-      </c>
-      <c r="M7">
+      <c r="K21" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="L21">
         <v>50</v>
       </c>
-      <c r="N7">
+      <c r="M21">
+        <v>50</v>
+      </c>
+      <c r="N21" s="1">
         <v>0.9</v>
       </c>
-      <c r="O7">
+      <c r="O21" t="s">
+        <v>116</v>
+      </c>
+      <c r="P21" s="1">
         <v>0.02</v>
       </c>
-      <c r="P7" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q7">
-        <v>3</v>
-      </c>
-      <c r="R7">
-        <v>0.12</v>
-      </c>
-      <c r="S7" s="3">
-        <f t="shared" ref="S7:S8" si="1">863*12</f>
-        <v>10356</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" t="b">
+      <c r="Q21">
         <v>0</v>
       </c>
-      <c r="J8" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="K8" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="L8">
-        <v>50</v>
-      </c>
-      <c r="M8">
-        <v>50</v>
-      </c>
-      <c r="N8">
-        <v>0.9</v>
-      </c>
-      <c r="O8">
-        <v>0.02</v>
-      </c>
-      <c r="P8" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q8">
+      <c r="R21" t="s">
+        <v>11</v>
+      </c>
+      <c r="S21">
         <v>1</v>
       </c>
-      <c r="R8">
-        <v>0.11</v>
-      </c>
-      <c r="S8" s="3">
+      <c r="T21" s="24">
+        <v>0</v>
+      </c>
+      <c r="U21" s="3">
         <f t="shared" si="1"/>
         <v>10356</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="S9" s="3"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" t="b">
-        <v>0</v>
-      </c>
-      <c r="S10" s="3"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" t="b">
-        <v>0</v>
-      </c>
-      <c r="S11" s="3"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" t="b">
-        <v>0</v>
-      </c>
-      <c r="S12" s="3"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>0.05</v>
-      </c>
-      <c r="H14">
-        <v>0.05</v>
-      </c>
-      <c r="I14">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" t="s">
-        <v>82</v>
-      </c>
-      <c r="D15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F15" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>0.05</v>
-      </c>
-      <c r="H15">
-        <v>0.05</v>
-      </c>
-      <c r="I15">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>80</v>
-      </c>
-      <c r="B16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" t="s">
-        <v>83</v>
-      </c>
-      <c r="D16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" t="b">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>0.06</v>
-      </c>
-      <c r="H16">
-        <v>0.06</v>
-      </c>
-      <c r="I16">
-        <v>6.5000000000000002E-2</v>
+      <c r="V21" s="1">
+        <v>0.11</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624C999D-0C1D-4D21-8244-0320CD22B8F8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1368,7 +2017,7 @@
   <dimension ref="B16:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:B28"/>
+      <selection activeCell="B20" sqref="B20:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1381,19 +2030,19 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G16" t="s">
         <v>5</v>
       </c>
       <c r="H16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I16" t="s">
         <v>3</v>
@@ -1402,10 +2051,10 @@
         <v>4</v>
       </c>
       <c r="K16" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="M16" t="s">
         <v>6</v>
@@ -1431,7 +2080,7 @@
         <v>0.02</v>
       </c>
       <c r="G17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H17">
         <v>57</v>
@@ -1446,7 +2095,7 @@
         <v>3</v>
       </c>
       <c r="N17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
@@ -1454,10 +2103,10 @@
         <v>8</v>
       </c>
       <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
         <v>14</v>
-      </c>
-      <c r="D18" t="s">
-        <v>15</v>
       </c>
       <c r="E18">
         <v>2.5000000000000001E-2</v>
@@ -1466,7 +2115,7 @@
         <v>0.02</v>
       </c>
       <c r="G18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H18">
         <v>57</v>
@@ -1481,7 +2130,7 @@
         <v>3</v>
       </c>
       <c r="N18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
@@ -1489,10 +2138,10 @@
         <v>8</v>
       </c>
       <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
         <v>16</v>
-      </c>
-      <c r="D19" t="s">
-        <v>17</v>
       </c>
       <c r="E19">
         <v>0.03</v>
@@ -1501,7 +2150,7 @@
         <v>0.02</v>
       </c>
       <c r="G19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H19">
         <v>50</v>
@@ -1516,18 +2165,18 @@
         <v>3</v>
       </c>
       <c r="N19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E20">
         <v>0.02</v>
@@ -1536,7 +2185,7 @@
         <v>0.02</v>
       </c>
       <c r="G20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H20">
         <v>57</v>
@@ -1545,18 +2194,18 @@
         <v>55</v>
       </c>
       <c r="N20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E21">
         <v>1.4999999999999999E-2</v>
@@ -1565,7 +2214,7 @@
         <v>0.02</v>
       </c>
       <c r="G21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H21">
         <v>57</v>
@@ -1574,32 +2223,32 @@
         <v>55</v>
       </c>
       <c r="N21" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1626,24 +2275,24 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
       <c r="D2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1660,7 +2309,7 @@
         <v>2799.16</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2859,32 +3508,32 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -3780,7 +4429,7 @@
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -3805,50 +4454,50 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -3860,4 +4509,381 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9076845A-E50F-429A-A005-D0BDC1AEFB3D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{304A5010-D7F4-42F6-8020-6F687E3F45AA}">
+  <dimension ref="A2:F44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="50.77734375" customWidth="1"/>
+    <col min="2" max="2" width="53.109375" customWidth="1"/>
+    <col min="3" max="3" width="38.21875" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" customWidth="1"/>
+    <col min="5" max="5" width="37.6640625" customWidth="1"/>
+    <col min="6" max="6" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="20"/>
+    </row>
+    <row r="8" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="14"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D11" s="14"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="14"/>
+    </row>
+    <row r="19" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="14"/>
+    </row>
+    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" s="14"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="14"/>
+      <c r="C21" s="14"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="14"/>
+      <c r="C22" s="14"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="14"/>
+      <c r="C23" s="14"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="14"/>
+      <c r="C24" s="14"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="14"/>
+      <c r="C25" s="14"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="14"/>
+      <c r="C26" s="14"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="14"/>
+      <c r="C27" s="14"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B29" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1.4500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="3">
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" s="2">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{1E3F88C6-CFF1-43D7-A3D4-02A1039B836B}"/>
+    <hyperlink ref="B8" r:id="rId2" xr:uid="{A6BB754D-61B3-4988-B7E2-A137270B7445}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{091E43DB-7AAF-44F1-B4B9-61F28ACF5A2E}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{FD649B16-454F-425E-ABF3-2DD4DBAF2EBD}"/>
+    <hyperlink ref="B19" r:id="rId5" display="http://www.massretirees.com/article/issues/cola/cola-base-and-its-history" xr:uid="{D246BC47-05CB-4FA1-8415-5E822B4D178C}"/>
+    <hyperlink ref="A6" r:id="rId6" xr:uid="{41F34DAF-EF08-4AC0-A774-6EFED58B8B47}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId7"/>
+  <drawing r:id="rId8"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAADA4E6-2532-4850-9BD3-D539B0F9EE03}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B4DE83-0AB8-4B16-BEC1-BCD5CAFBB3DE}">
+  <dimension ref="A2:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" s="22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" s="22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>